<commit_message>
Actualización del proyecto: agregando analysys_notebook, mejora documentario, eliminar grafias exepcion
</commit_message>
<xml_diff>
--- a/DataBase/productos.xlsx
+++ b/DataBase/productos.xlsx
@@ -345,7 +345,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +357,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -398,8 +404,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1760,7 +1766,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -1788,7 +1794,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>4286</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -1816,7 +1822,7 @@
         <v>4778</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>4289</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -1872,7 +1878,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>2394</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -1900,7 +1906,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -1942,7 +1948,7 @@
         <v>4090</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>2902</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>4690</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>4920</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>872</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>2843</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -2138,25 +2144,25 @@
         <v>4854</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="4"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>

</xml_diff>